<commit_message>
More updates to how maturity is calculated.
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_240102.xlsx
+++ b/data/hake_intrasp_240102.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC33CA1F-4F41-9144-9022-9D8E2EBEC5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7061FB6-4EF5-2446-8699-ED130F1FA45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35820" yWindow="-3400" windowWidth="29300" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="500" windowWidth="26640" windowHeight="20500" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -4044,7 +4044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AI271"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A182" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A164" sqref="A164"/>
     </sheetView>
   </sheetViews>
@@ -24964,7 +24964,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25039,13 +25039,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -29986,8 +29986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -30094,7 +30094,7 @@
         <v>53</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -33111,7 +33111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -33368,7 +33368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated nselages to match assessment
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_240102.xlsx
+++ b/data/hake_intrasp_240102.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7061FB6-4EF5-2446-8699-ED130F1FA45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4D373E-0774-A44B-B38F-CE2CDAFB76CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="500" windowWidth="26640" windowHeight="20500" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="500" windowWidth="26640" windowHeight="20500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1622,7 +1622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="D16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -33111,8 +33111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -33249,7 +33249,7 @@
         <v>5</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -33305,7 +33305,7 @@
         <v>5</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -33368,7 +33368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>

</xml_diff>